<commit_message>
Update Kenya DHA and EPA
</commit_message>
<xml_diff>
--- a/data/raw/Kenya/kenya_ingredients_dha_epa.xlsx
+++ b/data/raw/Kenya/kenya_ingredients_dha_epa.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisunjae/Documents/Activities/Golden Research/subnational_distributions/data/raw/Kenya/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E2A12CC8-65C5-6B41-A865-54D1FD541BBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E38557-C984-2C41-9F2F-91D3AF4B81E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="10920" windowWidth="26040" windowHeight="14940"/>
+    <workbookView xWindow="5260" yWindow="10920" windowWidth="26040" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kenya_ingredients" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.###;;"/>
   </numFmts>
@@ -1111,11 +1111,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:G28"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1307,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>D8+E8</f>
+        <f t="shared" ref="F8:F16" si="1">D8+E8</f>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="G8" t="s">
@@ -1331,7 +1331,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>D9+E9</f>
+        <f t="shared" si="1"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G9" t="s">
@@ -1355,7 +1355,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>D10+E10</f>
+        <f t="shared" si="1"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G10" t="s">
@@ -1379,7 +1379,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>D11+E11</f>
+        <f t="shared" si="1"/>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="G11" t="s">
@@ -1403,7 +1403,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>D12+E12</f>
+        <f t="shared" si="1"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G12" t="s">
@@ -1427,7 +1427,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>D13+E13</f>
+        <f t="shared" si="1"/>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="G13" t="s">
@@ -1451,7 +1451,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>D14+E14</f>
+        <f t="shared" si="1"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G14" t="s">
@@ -1475,7 +1475,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>D15+E15</f>
+        <f t="shared" si="1"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G15" t="s">
@@ -1499,7 +1499,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>D16+E16</f>
+        <f t="shared" si="1"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G16" t="s">
@@ -1523,7 +1523,7 @@
         <v>0.219</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" ref="F17:F20" si="1">D17+E17</f>
+        <f t="shared" ref="F17:F20" si="2">D17+E17</f>
         <v>0.318</v>
       </c>
       <c r="G17" t="s">
@@ -1547,7 +1547,7 @@
         <v>0.219</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.318</v>
       </c>
       <c r="G18" t="s">
@@ -1571,7 +1571,7 @@
         <v>0.219</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.318</v>
       </c>
       <c r="G19" t="s">
@@ -1595,7 +1595,7 @@
         <v>0.219</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.318</v>
       </c>
       <c r="G20" t="s">
@@ -1619,7 +1619,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>D21+E21</f>
+        <f t="shared" ref="F21:F48" si="3">D21+E21</f>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G21" t="s">
@@ -1643,7 +1643,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>D22+E22</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G22" t="s">
@@ -1667,7 +1667,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>D23+E23</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G23" t="s">
@@ -1691,7 +1691,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>D24+E24</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G24" t="s">
@@ -1715,7 +1715,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>D25+E25</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G25" t="s">
@@ -1739,7 +1739,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>D26+E26</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G26" t="s">
@@ -1763,7 +1763,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>D27+E27</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G27" t="s">
@@ -1787,7 +1787,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>D28+E28</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G28" t="s">
@@ -1811,7 +1811,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>D29+E29</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G29" t="s">
@@ -1835,7 +1835,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>D30+E30</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G30" t="s">
@@ -1859,7 +1859,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="F31" s="1">
-        <f>D31+E31</f>
+        <f t="shared" si="3"/>
         <v>0.17599999999999999</v>
       </c>
       <c r="G31" t="s">
@@ -1883,7 +1883,7 @@
         <v>0.114</v>
       </c>
       <c r="F32" s="1">
-        <f>D32+E32</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G32" t="s">
@@ -1907,7 +1907,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F33" s="1">
-        <f>D33+E33</f>
+        <f t="shared" si="3"/>
         <v>0.44199999999999995</v>
       </c>
       <c r="G33" t="s">
@@ -1931,7 +1931,7 @@
         <v>0.114</v>
       </c>
       <c r="F34" s="1">
-        <f>D34+E34</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G34" t="s">
@@ -1955,7 +1955,7 @@
         <v>0.114</v>
       </c>
       <c r="F35" s="1">
-        <f>D35+E35</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G35" t="s">
@@ -1979,7 +1979,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F36" s="1">
-        <f>D36+E36</f>
+        <f t="shared" si="3"/>
         <v>0.44199999999999995</v>
       </c>
       <c r="G36" t="s">
@@ -2003,7 +2003,7 @@
         <v>0.114</v>
       </c>
       <c r="F37" s="1">
-        <f>D37+E37</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G37" t="s">
@@ -2027,7 +2027,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F38" s="1">
-        <f>D38+E38</f>
+        <f t="shared" si="3"/>
         <v>0.44199999999999995</v>
       </c>
       <c r="G38" t="s">
@@ -2051,7 +2051,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F39" s="1">
-        <f>D39+E39</f>
+        <f t="shared" si="3"/>
         <v>0.44199999999999995</v>
       </c>
       <c r="G39" t="s">
@@ -2075,7 +2075,7 @@
         <v>0.114</v>
       </c>
       <c r="F40" s="1">
-        <f>D40+E40</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G40" t="s">
@@ -2099,7 +2099,7 @@
         <v>0.114</v>
       </c>
       <c r="F41" s="1">
-        <f>D41+E41</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G41" t="s">
@@ -2123,7 +2123,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F42" s="1">
-        <f>D42+E42</f>
+        <f t="shared" si="3"/>
         <v>0.44199999999999995</v>
       </c>
       <c r="G42" t="s">
@@ -2147,7 +2147,7 @@
         <v>0.114</v>
       </c>
       <c r="F43" s="1">
-        <f>D43+E43</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G43" t="s">
@@ -2171,7 +2171,7 @@
         <v>0.114</v>
       </c>
       <c r="F44" s="1">
-        <f>D44+E44</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G44" t="s">
@@ -2195,7 +2195,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F45" s="1">
-        <f>D45+E45</f>
+        <f t="shared" si="3"/>
         <v>0.44199999999999995</v>
       </c>
       <c r="G45" t="s">
@@ -2219,7 +2219,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F46" s="1">
-        <f>D46+E46</f>
+        <f t="shared" si="3"/>
         <v>0.44199999999999995</v>
       </c>
       <c r="G46" t="s">
@@ -2243,7 +2243,7 @@
         <v>0.114</v>
       </c>
       <c r="F47" s="1">
-        <f>D47+E47</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G47" t="s">
@@ -2267,7 +2267,7 @@
         <v>0.114</v>
       </c>
       <c r="F48" s="1">
-        <f>D48+E48</f>
+        <f t="shared" si="3"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="G48" t="s">

</xml_diff>